<commit_message>
New Changes made has been committed including data driven framework
</commit_message>
<xml_diff>
--- a/LennoxMavenProject/LennoxMaven/inputdata.xlsx
+++ b/LennoxMavenProject/LennoxMaven/inputdata.xlsx
@@ -464,8 +464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -533,7 +533,7 @@
         <v>54321</v>
       </c>
       <c r="I2" s="2">
-        <v>36540</v>
+        <v>35079</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -562,7 +562,7 @@
         <v>45321</v>
       </c>
       <c r="I3" s="2">
-        <v>31441</v>
+        <v>29596</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -591,7 +591,7 @@
         <v>32145</v>
       </c>
       <c r="I4" s="2">
-        <v>37287</v>
+        <v>28136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>